<commit_message>
Some minor updates to testing
</commit_message>
<xml_diff>
--- a/fixtures/tables_test.xlsx
+++ b/fixtures/tables_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\spreadsheet-analyser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\data-import\fixtures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DE7CEB6-C448-426C-B5E0-9772611F42D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7B987D-B55F-4BDB-B2AA-0BB588AA4676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{595DF58D-7019-4BA2-9B27-5736C61F48C3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{595DF58D-7019-4BA2-9B27-5736C61F48C3}"/>
   </bookViews>
   <sheets>
     <sheet name="Standard" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="24">
   <si>
     <t>Vitality</t>
   </si>
@@ -164,7 +164,71 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="35">
+  <dxfs count="52">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF90FF90"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FF90FF90"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -309,54 +373,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C380D2E8-DF22-48FC-A0E8-DA506CDC9B8A}" name="Soldier" displayName="Soldier" ref="A1:I21" dataDxfId="34">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C380D2E8-DF22-48FC-A0E8-DA506CDC9B8A}" name="Soldier" displayName="Soldier" ref="A1:I21" dataDxfId="51">
   <autoFilter ref="A1:I21" xr:uid="{C380D2E8-DF22-48FC-A0E8-DA506CDC9B8A}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D2133BA1-3125-483B-B4B3-1D44E615FB47}" name="Level" totalsRowLabel="Total"/>
-    <tableColumn id="2" xr3:uid="{2D633595-77A3-49AC-B1A4-F9428423794C}" name="Vitality" dataDxfId="33" totalsRowDxfId="32"/>
-    <tableColumn id="3" xr3:uid="{7156F64F-DA79-42F7-AFFC-391454448658}" name="Attack" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="4" xr3:uid="{779F68FB-5E06-4E31-B598-8BF7787B64C8}" name="Defence" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{B04137D2-F345-4EC8-AE92-244F57B7A077}" name="Fortitude" dataDxfId="27" totalsRowDxfId="26"/>
-    <tableColumn id="6" xr3:uid="{C84AC09C-2FD6-4D96-89A4-1AAAB1872F8D}" name="Reflex" dataDxfId="25" totalsRowDxfId="24"/>
-    <tableColumn id="7" xr3:uid="{95B834D8-DFEC-45F0-96FE-8371CB4B6D1F}" name="Will" dataDxfId="23" totalsRowDxfId="22"/>
-    <tableColumn id="8" xr3:uid="{521C6D33-BD77-4DEF-B2EB-4B45B278D553}" name="Feats granted" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{24B592BB-1DA6-433E-AEB7-2732785D99CF}" name="Feat" totalsRowFunction="count" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{2D633595-77A3-49AC-B1A4-F9428423794C}" name="Vitality" dataDxfId="50" totalsRowDxfId="49"/>
+    <tableColumn id="3" xr3:uid="{7156F64F-DA79-42F7-AFFC-391454448658}" name="Attack" dataDxfId="48" totalsRowDxfId="47"/>
+    <tableColumn id="4" xr3:uid="{779F68FB-5E06-4E31-B598-8BF7787B64C8}" name="Defence" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="5" xr3:uid="{B04137D2-F345-4EC8-AE92-244F57B7A077}" name="Fortitude" dataDxfId="44" totalsRowDxfId="43"/>
+    <tableColumn id="6" xr3:uid="{C84AC09C-2FD6-4D96-89A4-1AAAB1872F8D}" name="Reflex" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="7" xr3:uid="{95B834D8-DFEC-45F0-96FE-8371CB4B6D1F}" name="Will" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="8" xr3:uid="{521C6D33-BD77-4DEF-B2EB-4B45B278D553}" name="Feats granted" dataDxfId="38" totalsRowDxfId="37"/>
+    <tableColumn id="9" xr3:uid="{24B592BB-1DA6-433E-AEB7-2732785D99CF}" name="Feat" totalsRowFunction="count" dataDxfId="36" totalsRowDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5C2696C-5371-4E67-B0FE-A8CBA651A6A4}" name="Scout" displayName="Scout" ref="A23:I43" totalsRowShown="0" dataDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5C2696C-5371-4E67-B0FE-A8CBA651A6A4}" name="Scout" displayName="Scout" ref="A23:I43" totalsRowShown="0" dataDxfId="34">
   <autoFilter ref="A23:I43" xr:uid="{D5C2696C-5371-4E67-B0FE-A8CBA651A6A4}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{4E885477-E090-4EA0-833A-909E11C5D88A}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{8736D23A-CD5F-4B59-966D-7160C0CFB93B}" name="Vitality" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{1BCCF839-C720-4F71-81A9-20E0EFEC89BE}" name="Attack" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{D3BA732D-523B-41C6-965E-CDE17A3B0E57}" name="Defence" dataDxfId="14"/>
-    <tableColumn id="5" xr3:uid="{4957E15E-2A06-4085-A1BB-169114F8D4B0}" name="Fortitude" dataDxfId="13"/>
-    <tableColumn id="6" xr3:uid="{13E50AF9-6585-456D-AE23-CA1FFDF600A3}" name="Reflex" dataDxfId="12"/>
-    <tableColumn id="7" xr3:uid="{88E9E52A-505E-4411-9ABE-A189A3D319FC}" name="Will" dataDxfId="11"/>
-    <tableColumn id="8" xr3:uid="{2705D2D4-372E-4DD0-96C8-C3905C5E8211}" name="Feats granted" dataDxfId="10"/>
-    <tableColumn id="9" xr3:uid="{2B83293D-FE3F-4DB9-8169-48DF058C9321}" name="Feat" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{8736D23A-CD5F-4B59-966D-7160C0CFB93B}" name="Vitality" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{1BCCF839-C720-4F71-81A9-20E0EFEC89BE}" name="Attack" dataDxfId="32"/>
+    <tableColumn id="4" xr3:uid="{D3BA732D-523B-41C6-965E-CDE17A3B0E57}" name="Defence" dataDxfId="31"/>
+    <tableColumn id="5" xr3:uid="{4957E15E-2A06-4085-A1BB-169114F8D4B0}" name="Fortitude" dataDxfId="30"/>
+    <tableColumn id="6" xr3:uid="{13E50AF9-6585-456D-AE23-CA1FFDF600A3}" name="Reflex" dataDxfId="29"/>
+    <tableColumn id="7" xr3:uid="{88E9E52A-505E-4411-9ABE-A189A3D319FC}" name="Will" dataDxfId="28"/>
+    <tableColumn id="8" xr3:uid="{2705D2D4-372E-4DD0-96C8-C3905C5E8211}" name="Feats granted" dataDxfId="27"/>
+    <tableColumn id="9" xr3:uid="{2B83293D-FE3F-4DB9-8169-48DF058C9321}" name="Feat" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4ED78190-6EB9-40DD-A110-F174F3523B7E}" name="Scoundrel" displayName="Scoundrel" ref="A45:I65" totalsRowShown="0" dataDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4ED78190-6EB9-40DD-A110-F174F3523B7E}" name="Scoundrel" displayName="Scoundrel" ref="A45:I65" totalsRowShown="0" dataDxfId="25">
   <autoFilter ref="A45:I65" xr:uid="{4ED78190-6EB9-40DD-A110-F174F3523B7E}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{6792758F-C864-402E-83E7-373A9D697863}" name="Level"/>
-    <tableColumn id="2" xr3:uid="{3F556CD8-EB2E-4EB4-BDF1-2CC9A5BEF100}" name="Vitality" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{A409131B-5CA8-4FBE-A4E2-95F05C1765BD}" name="Attack" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{426036C8-4405-43E7-B286-8DB62D920885}" name="Defence" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{1987FC10-6859-4841-AF9E-4CCB4D2DF654}" name="Fortitude" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{1119867B-EFE8-4123-8430-C640406865EC}" name="Reflex" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{549EFBE7-5C31-4017-9FBF-E9EEE9F39CCF}" name="Will" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{81F1B2DF-FE69-48BE-B675-A8C4020AB126}" name="Feats granted" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{DBC55A6A-D799-4594-9EB9-B32FBD590C2E}" name="Feat" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{3F556CD8-EB2E-4EB4-BDF1-2CC9A5BEF100}" name="Vitality" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{A409131B-5CA8-4FBE-A4E2-95F05C1765BD}" name="Attack" dataDxfId="23"/>
+    <tableColumn id="4" xr3:uid="{426036C8-4405-43E7-B286-8DB62D920885}" name="Defence" dataDxfId="22"/>
+    <tableColumn id="5" xr3:uid="{1987FC10-6859-4841-AF9E-4CCB4D2DF654}" name="Fortitude" dataDxfId="21"/>
+    <tableColumn id="6" xr3:uid="{1119867B-EFE8-4123-8430-C640406865EC}" name="Reflex" dataDxfId="20"/>
+    <tableColumn id="7" xr3:uid="{549EFBE7-5C31-4017-9FBF-E9EEE9F39CCF}" name="Will" dataDxfId="19"/>
+    <tableColumn id="8" xr3:uid="{81F1B2DF-FE69-48BE-B675-A8C4020AB126}" name="Feats granted" dataDxfId="18"/>
+    <tableColumn id="9" xr3:uid="{DBC55A6A-D799-4594-9EB9-B32FBD590C2E}" name="Feat" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{94D54138-CD71-40B2-A497-354F059462E9}" name="Test1" displayName="Test1" ref="A1:I21" dataDxfId="16">
+  <autoFilter ref="A1:I21" xr:uid="{94D54138-CD71-40B2-A497-354F059462E9}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{C62D5372-E645-4390-A90D-64F715452B54}" name="Level" totalsRowLabel="Total"/>
+    <tableColumn id="2" xr3:uid="{B8BFD536-CACA-420B-8A96-51164CFF1030}" name="Vitality" dataDxfId="14" totalsRowDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{1644D532-656C-4602-B865-8323FA3E5968}" name="Attack" dataDxfId="12" totalsRowDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{C980A1CA-8F38-4CB5-97CE-9374A2A6FA62}" name="Defence" dataDxfId="10" totalsRowDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{FCAF6D1C-64E1-4773-8A64-B0A9B8A26A26}" name="Fortitude" dataDxfId="8" totalsRowDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{17E37B99-35A9-4E00-BCA4-3A2FA6D3CDF6}" name="Reflex" dataDxfId="6" totalsRowDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{389B88BD-B3CF-45CB-A03E-52D5A7431410}" name="Will" dataDxfId="4" totalsRowDxfId="5"/>
+    <tableColumn id="8" xr3:uid="{67D887BF-84C1-4A97-AAEB-459253382DBC}" name="Feats granted" dataDxfId="2" totalsRowDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{4F6B1797-76B9-41B9-A845-01C659250734}" name="Feat" totalsRowFunction="count" dataDxfId="0" totalsRowDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -661,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88F162AB-FD72-4E99-8392-DB88BB7E9966}">
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2304,14 +2386,547 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7C6A16A-86A3-4577-837B-793E7E1EDEF3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1">
+        <v>20</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1">
+        <v>3</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1">
+        <v>1</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1">
+        <v>4</v>
+      </c>
+      <c r="F6" s="5">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1"/>
+      <c r="I6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>60</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1">
+        <v>2</v>
+      </c>
+      <c r="H7" s="1"/>
+      <c r="I7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>70</v>
+      </c>
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5">
+        <v>2</v>
+      </c>
+      <c r="G8" s="1">
+        <v>2</v>
+      </c>
+      <c r="H8" s="1"/>
+      <c r="I8" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1">
+        <v>80</v>
+      </c>
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1">
+        <v>6</v>
+      </c>
+      <c r="F9" s="5">
+        <v>2</v>
+      </c>
+      <c r="G9" s="1">
+        <v>2</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1">
+        <v>90</v>
+      </c>
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1">
+        <v>6</v>
+      </c>
+      <c r="F10" s="5">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1">
+        <v>3</v>
+      </c>
+      <c r="H10" s="1"/>
+      <c r="I10" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1">
+        <v>100</v>
+      </c>
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1">
+        <v>7</v>
+      </c>
+      <c r="F11" s="5">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1">
+        <v>3</v>
+      </c>
+      <c r="H11" s="1"/>
+      <c r="I11" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1">
+        <v>110</v>
+      </c>
+      <c r="C12" s="1">
+        <v>11</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1">
+        <v>7</v>
+      </c>
+      <c r="F12" s="5">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1">
+        <v>3</v>
+      </c>
+      <c r="H12" s="1"/>
+      <c r="I12" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>120</v>
+      </c>
+      <c r="C13" s="1">
+        <v>12</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1">
+        <v>8</v>
+      </c>
+      <c r="F13" s="5">
+        <v>4</v>
+      </c>
+      <c r="G13" s="1">
+        <v>4</v>
+      </c>
+      <c r="H13" s="1"/>
+      <c r="I13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1">
+        <v>130</v>
+      </c>
+      <c r="C14" s="1">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1">
+        <v>8</v>
+      </c>
+      <c r="F14" s="5">
+        <v>4</v>
+      </c>
+      <c r="G14" s="1">
+        <v>4</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1">
+        <v>140</v>
+      </c>
+      <c r="C15" s="1">
+        <v>14</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1">
+        <v>9</v>
+      </c>
+      <c r="F15" s="5">
+        <v>4</v>
+      </c>
+      <c r="G15" s="1">
+        <v>4</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1">
+        <v>150</v>
+      </c>
+      <c r="C16" s="1">
+        <v>15</v>
+      </c>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1">
+        <v>9</v>
+      </c>
+      <c r="F16" s="5">
+        <v>5</v>
+      </c>
+      <c r="G16" s="1">
+        <v>5</v>
+      </c>
+      <c r="H16" s="1"/>
+      <c r="I16" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1">
+        <v>160</v>
+      </c>
+      <c r="C17" s="1">
+        <v>16</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1">
+        <v>10</v>
+      </c>
+      <c r="F17" s="5">
+        <v>5</v>
+      </c>
+      <c r="G17" s="1">
+        <v>5</v>
+      </c>
+      <c r="H17" s="1"/>
+      <c r="I17" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1">
+        <v>170</v>
+      </c>
+      <c r="C18" s="1">
+        <v>17</v>
+      </c>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1">
+        <v>10</v>
+      </c>
+      <c r="F18" s="5">
+        <v>5</v>
+      </c>
+      <c r="G18" s="1">
+        <v>5</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1">
+        <v>180</v>
+      </c>
+      <c r="C19" s="1">
+        <v>18</v>
+      </c>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1">
+        <v>11</v>
+      </c>
+      <c r="F19" s="5">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1">
+        <v>6</v>
+      </c>
+      <c r="H19" s="1"/>
+      <c r="I19" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1">
+        <v>190</v>
+      </c>
+      <c r="C20" s="1">
+        <v>19</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1">
+        <v>11</v>
+      </c>
+      <c r="F20" s="5">
+        <v>6</v>
+      </c>
+      <c r="G20" s="1">
+        <v>6</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1">
+        <v>200</v>
+      </c>
+      <c r="C21" s="1">
+        <v>20</v>
+      </c>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1">
+        <v>12</v>
+      </c>
+      <c r="F21" s="5">
+        <v>6</v>
+      </c>
+      <c r="G21" s="1">
+        <v>6</v>
+      </c>
+      <c r="H21" s="1"/>
+      <c r="I21" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>